<commit_message>
agregado titulos de ejes en graficos
</commit_message>
<xml_diff>
--- a/analisis/Documentacion_coloreo.xlsx
+++ b/analisis/Documentacion_coloreo.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr hidePivotFieldList="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patricia\Dropbox\CUATRI22017\Avanzada\TP4GRAFOS\analisis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="7650" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="40% adyacencia" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="50% adyacencia" sheetId="4" r:id="rId4"/>
     <sheet name="75% de adyacencia" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,9 +141,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -175,7 +180,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -276,7 +280,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7FBC-4D15-AA65-DFF93EB47B3B}"/>
             </c:ext>
@@ -367,7 +371,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7FBC-4D15-AA65-DFF93EB47B3B}"/>
             </c:ext>
@@ -452,7 +456,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7FBC-4D15-AA65-DFF93EB47B3B}"/>
             </c:ext>
@@ -491,6 +495,29 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-AR" baseline="0"/>
+                  <a:t> de colores</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -553,6 +580,29 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Frecuencia</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-AR" baseline="0"/>
+                  <a:t> relativa</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -604,7 +654,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -672,9 +721,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -716,7 +765,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -835,7 +883,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EE3A-4B1E-A99E-489CDF9543A8}"/>
             </c:ext>
@@ -944,7 +992,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EE3A-4B1E-A99E-489CDF9543A8}"/>
             </c:ext>
@@ -1041,7 +1089,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-EE3A-4B1E-A99E-489CDF9543A8}"/>
             </c:ext>
@@ -1079,6 +1127,24 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad de colores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1141,6 +1207,29 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Frecuencia</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-AR" baseline="0"/>
+                  <a:t> relativa</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1192,7 +1281,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1233,9 +1321,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1272,7 +1360,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1421,7 +1508,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7FBB-45AC-B697-34A9C7EBF3C4}"/>
             </c:ext>
@@ -1566,7 +1653,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7FBB-45AC-B697-34A9C7EBF3C4}"/>
             </c:ext>
@@ -1687,7 +1774,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7FBB-45AC-B697-34A9C7EBF3C4}"/>
             </c:ext>
@@ -1725,6 +1812,24 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad colores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1787,6 +1892,24 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Frecuencia relativa</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1838,7 +1961,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1906,9 +2028,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1943,7 +2065,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2067,7 +2188,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BCB0-4E86-8C70-C945A7038977}"/>
             </c:ext>
@@ -2194,7 +2315,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-BCB0-4E86-8C70-C945A7038977}"/>
             </c:ext>
@@ -2327,7 +2448,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-BCB0-4E86-8C70-C945A7038977}"/>
             </c:ext>
@@ -2365,6 +2486,24 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad de colores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2427,6 +2566,24 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Frecuencia relativa</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2478,7 +2635,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2546,9 +2702,9 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2580,7 +2736,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2692,7 +2847,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0EE9-4BF9-A14D-3092E3D85C98}"/>
             </c:ext>
@@ -2801,7 +2956,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0EE9-4BF9-A14D-3092E3D85C98}"/>
             </c:ext>
@@ -2910,7 +3065,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0EE9-4BF9-A14D-3092E3D85C98}"/>
             </c:ext>
@@ -2948,6 +3103,24 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad de colores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3010,6 +3183,24 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Frecuencia relativa</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3061,7 +3252,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3145,7 +3335,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3180,7 +3376,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3215,7 +3417,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3250,7 +3458,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3285,7 +3499,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3558,18 +3778,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3718,7 +3938,7 @@
         <v>61</v>
       </c>
       <c r="H15" s="3">
-        <f>I15/$H$22</f>
+        <f t="shared" ref="H15:H21" si="1">I15/$H$22</f>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I15" s="3">
@@ -3730,7 +3950,7 @@
         <v>62</v>
       </c>
       <c r="H16" s="3">
-        <f>I16/$H$22</f>
+        <f t="shared" si="1"/>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="I16" s="3">
@@ -3742,7 +3962,7 @@
         <v>63</v>
       </c>
       <c r="H17" s="3">
-        <f>I17/$H$22</f>
+        <f t="shared" si="1"/>
         <v>0.22</v>
       </c>
       <c r="I17" s="3">
@@ -3754,7 +3974,7 @@
         <v>64</v>
       </c>
       <c r="H18" s="3">
-        <f>I18/$H$22</f>
+        <f t="shared" si="1"/>
         <v>0.36599999999999999</v>
       </c>
       <c r="I18" s="3">
@@ -3766,7 +3986,7 @@
         <v>65</v>
       </c>
       <c r="H19" s="3">
-        <f>I19/$H$22</f>
+        <f t="shared" si="1"/>
         <v>0.25700000000000001</v>
       </c>
       <c r="I19" s="3">
@@ -3778,7 +3998,7 @@
         <v>66</v>
       </c>
       <c r="H20" s="3">
-        <f>I20/$H$22</f>
+        <f t="shared" si="1"/>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="I20" s="3">
@@ -3790,7 +4010,7 @@
         <v>67</v>
       </c>
       <c r="H21" s="3">
-        <f>I21/$H$22</f>
+        <f t="shared" si="1"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="I21" s="3">
@@ -3839,7 +4059,7 @@
         <v>68</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" ref="H27:H33" si="1">I27/$H$34</f>
+        <f t="shared" ref="H27:H33" si="2">I27/$H$34</f>
         <v>0.11600000000000001</v>
       </c>
       <c r="I27" s="3">
@@ -3851,7 +4071,7 @@
         <v>69</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.30399999999999999</v>
       </c>
       <c r="I28" s="3">
@@ -3863,7 +4083,7 @@
         <v>70</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.32300000000000001</v>
       </c>
       <c r="I29" s="3">
@@ -3875,7 +4095,7 @@
         <v>71</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.185</v>
       </c>
       <c r="I30" s="3">
@@ -3887,7 +4107,7 @@
         <v>72</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="I31" s="3">
@@ -3899,7 +4119,7 @@
         <v>73</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="I32" s="3">
@@ -3911,7 +4131,7 @@
         <v>74</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="I33" s="3">
@@ -3938,11 +4158,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="F1:H42"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3972,7 +4192,7 @@
         <v>99</v>
       </c>
       <c r="G3" s="3">
-        <f>H3/$G$14</f>
+        <f t="shared" ref="G3:G13" si="0">H3/$G$14</f>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H3" s="3">
@@ -3984,7 +4204,7 @@
         <v>100</v>
       </c>
       <c r="G4" s="3">
-        <f>H4/$G$14</f>
+        <f t="shared" si="0"/>
         <v>2.3E-2</v>
       </c>
       <c r="H4" s="3">
@@ -3996,7 +4216,7 @@
         <v>101</v>
       </c>
       <c r="G5" s="3">
-        <f>H5/$G$14</f>
+        <f t="shared" si="0"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="H5" s="3">
@@ -4008,7 +4228,7 @@
         <v>102</v>
       </c>
       <c r="G6" s="3">
-        <f>H6/$G$14</f>
+        <f t="shared" si="0"/>
         <v>0.182</v>
       </c>
       <c r="H6" s="3">
@@ -4020,7 +4240,7 @@
         <v>103</v>
       </c>
       <c r="G7" s="3">
-        <f>H7/$G$14</f>
+        <f t="shared" si="0"/>
         <v>0.249</v>
       </c>
       <c r="H7" s="3">
@@ -4032,7 +4252,7 @@
         <v>104</v>
       </c>
       <c r="G8" s="3">
-        <f>H8/$G$14</f>
+        <f t="shared" si="0"/>
         <v>0.255</v>
       </c>
       <c r="H8" s="3">
@@ -4044,7 +4264,7 @@
         <v>105</v>
       </c>
       <c r="G9" s="3">
-        <f>H9/$G$14</f>
+        <f t="shared" si="0"/>
         <v>0.14199999999999999</v>
       </c>
       <c r="H9" s="3">
@@ -4056,7 +4276,7 @@
         <v>106</v>
       </c>
       <c r="G10" s="3">
-        <f>H10/$G$14</f>
+        <f t="shared" si="0"/>
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="H10" s="3">
@@ -4068,7 +4288,7 @@
         <v>107</v>
       </c>
       <c r="G11" s="3">
-        <f>H11/$G$14</f>
+        <f t="shared" si="0"/>
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H11" s="3">
@@ -4080,7 +4300,7 @@
         <v>108</v>
       </c>
       <c r="G12" s="3">
-        <f>H12/$G$14</f>
+        <f t="shared" si="0"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H12" s="3">
@@ -4092,7 +4312,7 @@
         <v>109</v>
       </c>
       <c r="G13" s="3">
-        <f>H13/$G$14</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="H13" s="3">
@@ -4126,7 +4346,7 @@
         <v>97</v>
       </c>
       <c r="G18" s="3">
-        <f>H18/$G$27</f>
+        <f t="shared" ref="G18:G26" si="1">H18/$G$27</f>
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="H18" s="3">
@@ -4138,7 +4358,7 @@
         <v>98</v>
       </c>
       <c r="G19" s="3">
-        <f>H19/$G$27</f>
+        <f t="shared" si="1"/>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="H19" s="3">
@@ -4150,7 +4370,7 @@
         <v>99</v>
       </c>
       <c r="G20" s="3">
-        <f>H20/$G$27</f>
+        <f t="shared" si="1"/>
         <v>0.159</v>
       </c>
       <c r="H20" s="3">
@@ -4162,7 +4382,7 @@
         <v>100</v>
       </c>
       <c r="G21" s="3">
-        <f>H21/$G$27</f>
+        <f t="shared" si="1"/>
         <v>0.249</v>
       </c>
       <c r="H21" s="3">
@@ -4174,7 +4394,7 @@
         <v>101</v>
       </c>
       <c r="G22" s="3">
-        <f>H22/$G$27</f>
+        <f t="shared" si="1"/>
         <v>0.30099999999999999</v>
       </c>
       <c r="H22" s="3">
@@ -4186,7 +4406,7 @@
         <v>102</v>
       </c>
       <c r="G23" s="3">
-        <f>H23/$G$27</f>
+        <f t="shared" si="1"/>
         <v>0.16600000000000001</v>
       </c>
       <c r="H23" s="3">
@@ -4198,7 +4418,7 @@
         <v>103</v>
       </c>
       <c r="G24" s="3">
-        <f>H24/$G$27</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="H24" s="3">
@@ -4210,7 +4430,7 @@
         <v>104</v>
       </c>
       <c r="G25" s="3">
-        <f>H25/$G$27</f>
+        <f t="shared" si="1"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="H25" s="3">
@@ -4222,7 +4442,7 @@
         <v>105</v>
       </c>
       <c r="G26" s="3">
-        <f>H26/$G$27</f>
+        <f t="shared" si="1"/>
         <v>1E-3</v>
       </c>
       <c r="H26" s="3">
@@ -4256,7 +4476,7 @@
         <v>102</v>
       </c>
       <c r="G31" s="3">
-        <f>H31/$G$42</f>
+        <f t="shared" ref="G31:G41" si="2">H31/$G$42</f>
         <v>1E-3</v>
       </c>
       <c r="H31" s="3">
@@ -4268,7 +4488,7 @@
         <v>103</v>
       </c>
       <c r="G32" s="3">
-        <f>H32/$G$42</f>
+        <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
       <c r="H32" s="3">
@@ -4280,7 +4500,7 @@
         <v>104</v>
       </c>
       <c r="G33" s="3">
-        <f>H33/$G$42</f>
+        <f t="shared" si="2"/>
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="H33" s="3">
@@ -4292,7 +4512,7 @@
         <v>105</v>
       </c>
       <c r="G34" s="3">
-        <f>H34/$G$42</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="H34" s="3">
@@ -4304,7 +4524,7 @@
         <v>106</v>
       </c>
       <c r="G35" s="3">
-        <f>H35/$G$42</f>
+        <f t="shared" si="2"/>
         <v>0.214</v>
       </c>
       <c r="H35" s="3">
@@ -4316,7 +4536,7 @@
         <v>107</v>
       </c>
       <c r="G36" s="3">
-        <f>H36/$G$42</f>
+        <f t="shared" si="2"/>
         <v>0.24299999999999999</v>
       </c>
       <c r="H36" s="3">
@@ -4328,7 +4548,7 @@
         <v>108</v>
       </c>
       <c r="G37" s="3">
-        <f>H37/$G$42</f>
+        <f t="shared" si="2"/>
         <v>0.219</v>
       </c>
       <c r="H37" s="3">
@@ -4340,7 +4560,7 @@
         <v>109</v>
       </c>
       <c r="G38" s="3">
-        <f>H38/$G$42</f>
+        <f t="shared" si="2"/>
         <v>0.106</v>
       </c>
       <c r="H38" s="3">
@@ -4352,7 +4572,7 @@
         <v>110</v>
       </c>
       <c r="G39" s="3">
-        <f>H39/$G$42</f>
+        <f t="shared" si="2"/>
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="H39" s="3">
@@ -4364,7 +4584,7 @@
         <v>111</v>
       </c>
       <c r="G40" s="3">
-        <f>H40/$G$42</f>
+        <f t="shared" si="2"/>
         <v>1.6E-2</v>
       </c>
       <c r="H40" s="3">
@@ -4376,7 +4596,7 @@
         <v>112</v>
       </c>
       <c r="G41" s="3">
-        <f>H41/$G$42</f>
+        <f t="shared" si="2"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H41" s="3">
@@ -4403,11 +4623,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="F1:H57"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:G39"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5049,11 +5269,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13555,11 +13775,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="F1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>